<commit_message>
Personalizando titulo de pestaña y favicon
</commit_message>
<xml_diff>
--- a/graduacion/graduacion.xlsx
+++ b/graduacion/graduacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/Desktop/ ANTIGRAVITY/graduacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405F67CF-45E1-3346-83CF-7F90BD9FF5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C2B6A4-4AA4-7943-A4B4-6BA090A672B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16140" xr2:uid="{0C5D4335-B98D-8C4A-B531-C3D387BAD24B}"/>
   </bookViews>
@@ -1189,7 +1189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F3CF557-8EC8-CD40-9C10-648C71E32AFF}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>

</xml_diff>